<commit_message>
Fixed Trigger & Jitter
Fixed issues related to jitter (i.e., selected columns 0:60, and attribute ITI to new scenes), test_trigger file that has working triggers to stimuli; some rephrasing of instructions and repositioning; added missing items to the stimuli dataset
</commit_message>
<xml_diff>
--- a/encode_pairs.xlsx
+++ b/encode_pairs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vera/Documents/GitHub/SEED/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DD42790-54A1-C948-9C68-A343975E5536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{004B3C56-13A9-0948-9391-63517AD27ADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41520" yWindow="940" windowWidth="17580" windowHeight="15220" xr2:uid="{3362159E-E323-D04B-86B0-C30BAC9B69B5}"/>
+    <workbookView xWindow="31120" yWindow="1720" windowWidth="16880" windowHeight="17500" xr2:uid="{3362159E-E323-D04B-86B0-C30BAC9B69B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -1216,7 +1216,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1228,7 +1228,6 @@
     <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1563,10 +1562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC9664D9-E733-C548-8E73-813AA8405C24}">
-  <dimension ref="A1:O94"/>
+  <dimension ref="A1:N91"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N62" sqref="N62:N97"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61:XFD61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1580,7 +1579,7 @@
     <col min="13" max="13" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>58</v>
       </c>
@@ -1624,7 +1623,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1667,11 +1666,8 @@
       <c r="N2">
         <v>2</v>
       </c>
-      <c r="O2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1714,11 +1710,8 @@
       <c r="N3">
         <v>2.0499999999999998</v>
       </c>
-      <c r="O3">
-        <v>2.0499999999999998</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1761,11 +1754,8 @@
       <c r="N4">
         <v>2.1</v>
       </c>
-      <c r="O4">
-        <v>2.1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1808,11 +1798,8 @@
       <c r="N5">
         <v>2.15</v>
       </c>
-      <c r="O5">
-        <v>2.15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1855,11 +1842,8 @@
       <c r="N6">
         <v>2.2000000000000002</v>
       </c>
-      <c r="O6">
-        <v>2.2000000000000002</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1902,11 +1886,8 @@
       <c r="N7">
         <v>2.25</v>
       </c>
-      <c r="O7">
-        <v>2.25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1949,11 +1930,8 @@
       <c r="N8">
         <v>2.2999999999999998</v>
       </c>
-      <c r="O8">
-        <v>2.2999999999999998</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1996,11 +1974,8 @@
       <c r="N9">
         <v>2.35</v>
       </c>
-      <c r="O9">
-        <v>2.35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2043,11 +2018,8 @@
       <c r="N10">
         <v>2.4</v>
       </c>
-      <c r="O10">
-        <v>2.4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2090,11 +2062,8 @@
       <c r="N11">
         <v>2.4500000000000002</v>
       </c>
-      <c r="O11">
-        <v>2.4500000000000002</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2137,11 +2106,8 @@
       <c r="N12">
         <v>2.5</v>
       </c>
-      <c r="O12">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2184,11 +2150,8 @@
       <c r="N13">
         <v>2.5499999999999998</v>
       </c>
-      <c r="O13">
-        <v>2.5499999999999998</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2231,11 +2194,8 @@
       <c r="N14">
         <v>2.6</v>
       </c>
-      <c r="O14">
-        <v>2.6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2278,11 +2238,8 @@
       <c r="N15">
         <v>2.65</v>
       </c>
-      <c r="O15">
-        <v>2.65</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2325,11 +2282,8 @@
       <c r="N16">
         <v>2.7</v>
       </c>
-      <c r="O16">
-        <v>2.7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2372,11 +2326,8 @@
       <c r="N17">
         <v>2.75</v>
       </c>
-      <c r="O17">
-        <v>2.75</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2419,11 +2370,8 @@
       <c r="N18">
         <v>2.8</v>
       </c>
-      <c r="O18">
-        <v>2.8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2466,11 +2414,8 @@
       <c r="N19">
         <v>2.85</v>
       </c>
-      <c r="O19">
-        <v>2.85</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2513,11 +2458,8 @@
       <c r="N20">
         <v>2.9</v>
       </c>
-      <c r="O20">
-        <v>2.9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2560,11 +2502,8 @@
       <c r="N21">
         <v>2.95</v>
       </c>
-      <c r="O21">
-        <v>2.95</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2607,11 +2546,8 @@
       <c r="N22">
         <v>3</v>
       </c>
-      <c r="O22">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2654,11 +2590,8 @@
       <c r="N23">
         <v>3.05</v>
       </c>
-      <c r="O23">
-        <v>3.05</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2701,11 +2634,8 @@
       <c r="N24">
         <v>3.1</v>
       </c>
-      <c r="O24">
-        <v>3.1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2748,11 +2678,8 @@
       <c r="N25">
         <v>3.15</v>
       </c>
-      <c r="O25">
-        <v>3.15</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2795,11 +2722,8 @@
       <c r="N26">
         <v>3.2</v>
       </c>
-      <c r="O26">
-        <v>3.2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2842,11 +2766,8 @@
       <c r="N27">
         <v>3.25</v>
       </c>
-      <c r="O27">
-        <v>3.25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2890,7 +2811,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2934,7 +2855,7 @@
         <v>2.0499999999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2978,7 +2899,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3022,7 +2943,7 @@
         <v>2.15</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -4358,6 +4279,9 @@
       <c r="E62" s="3" t="s">
         <v>362</v>
       </c>
+      <c r="N62">
+        <v>2</v>
+      </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63">
@@ -4375,6 +4299,9 @@
       <c r="E63" s="3" t="s">
         <v>362</v>
       </c>
+      <c r="N63">
+        <v>2.0499999999999998</v>
+      </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64">
@@ -4392,6 +4319,9 @@
       <c r="E64" s="3" t="s">
         <v>362</v>
       </c>
+      <c r="N64">
+        <v>2.1</v>
+      </c>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65">
@@ -4409,6 +4339,9 @@
       <c r="E65" s="3" t="s">
         <v>362</v>
       </c>
+      <c r="N65">
+        <v>2.15</v>
+      </c>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66">
@@ -4426,6 +4359,9 @@
       <c r="E66" s="3" t="s">
         <v>362</v>
       </c>
+      <c r="N66">
+        <v>2.2000000000000002</v>
+      </c>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67">
@@ -4443,6 +4379,9 @@
       <c r="E67" s="3" t="s">
         <v>362</v>
       </c>
+      <c r="N67">
+        <v>2.25</v>
+      </c>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68">
@@ -4460,6 +4399,9 @@
       <c r="E68" s="3" t="s">
         <v>362</v>
       </c>
+      <c r="N68">
+        <v>2.2999999999999998</v>
+      </c>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69">
@@ -4477,6 +4419,9 @@
       <c r="E69" s="3" t="s">
         <v>362</v>
       </c>
+      <c r="N69">
+        <v>2.35</v>
+      </c>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70">
@@ -4494,6 +4439,9 @@
       <c r="E70" s="3" t="s">
         <v>362</v>
       </c>
+      <c r="N70">
+        <v>2.4</v>
+      </c>
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A71">
@@ -4511,6 +4459,9 @@
       <c r="E71" s="3" t="s">
         <v>362</v>
       </c>
+      <c r="N71">
+        <v>2.4500000000000002</v>
+      </c>
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A72">
@@ -4528,6 +4479,9 @@
       <c r="E72" s="3" t="s">
         <v>362</v>
       </c>
+      <c r="N72">
+        <v>2.5</v>
+      </c>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A73">
@@ -4545,6 +4499,9 @@
       <c r="E73" s="3" t="s">
         <v>362</v>
       </c>
+      <c r="N73">
+        <v>2.5499999999999998</v>
+      </c>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74">
@@ -4562,6 +4519,9 @@
       <c r="E74" s="3" t="s">
         <v>362</v>
       </c>
+      <c r="N74">
+        <v>2.6</v>
+      </c>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75">
@@ -4579,6 +4539,9 @@
       <c r="E75" s="3" t="s">
         <v>362</v>
       </c>
+      <c r="N75">
+        <v>2.65</v>
+      </c>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76">
@@ -4596,6 +4559,9 @@
       <c r="E76" s="3" t="s">
         <v>362</v>
       </c>
+      <c r="N76">
+        <v>2.7</v>
+      </c>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77">
@@ -4613,6 +4579,9 @@
       <c r="E77" s="3" t="s">
         <v>362</v>
       </c>
+      <c r="N77">
+        <v>2.75</v>
+      </c>
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78">
@@ -4630,6 +4599,9 @@
       <c r="E78" s="3" t="s">
         <v>362</v>
       </c>
+      <c r="N78">
+        <v>2.8</v>
+      </c>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79">
@@ -4647,6 +4619,9 @@
       <c r="E79" s="3" t="s">
         <v>362</v>
       </c>
+      <c r="N79">
+        <v>2.85</v>
+      </c>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80">
@@ -4664,7 +4639,9 @@
       <c r="E80" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="N80" s="11"/>
+      <c r="N80">
+        <v>2.9</v>
+      </c>
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A81">
@@ -4682,7 +4659,9 @@
       <c r="E81" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="N81" s="11"/>
+      <c r="N81">
+        <v>2.95</v>
+      </c>
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A82">
@@ -4700,7 +4679,9 @@
       <c r="E82" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="N82" s="11"/>
+      <c r="N82">
+        <v>3</v>
+      </c>
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A83">
@@ -4718,7 +4699,9 @@
       <c r="E83" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="N83" s="11"/>
+      <c r="N83">
+        <v>3.05</v>
+      </c>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A84">
@@ -4736,7 +4719,9 @@
       <c r="E84" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="N84" s="11"/>
+      <c r="N84">
+        <v>3.1</v>
+      </c>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A85">
@@ -4754,7 +4739,9 @@
       <c r="E85" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="N85" s="11"/>
+      <c r="N85">
+        <v>3.15</v>
+      </c>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A86">
@@ -4772,7 +4759,9 @@
       <c r="E86" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="N86" s="11"/>
+      <c r="N86">
+        <v>3.2</v>
+      </c>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A87">
@@ -4790,7 +4779,9 @@
       <c r="E87" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="N87" s="11"/>
+      <c r="N87">
+        <v>3.25</v>
+      </c>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A88">
@@ -4808,7 +4799,9 @@
       <c r="E88" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="N88" s="11"/>
+      <c r="N88">
+        <v>2</v>
+      </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A89">
@@ -4826,7 +4819,9 @@
       <c r="E89" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="N89" s="11"/>
+      <c r="N89">
+        <v>2.0499999999999998</v>
+      </c>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A90">
@@ -4844,7 +4839,9 @@
       <c r="E90" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="N90" s="11"/>
+      <c r="N90">
+        <v>2.1</v>
+      </c>
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A91">
@@ -4862,16 +4859,9 @@
       <c r="E91" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="N91" s="11"/>
-    </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="N92" s="6"/>
-    </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="N93" s="6"/>
-    </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="N94" s="6"/>
+      <c r="N91">
+        <v>2.85</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>